<commit_message>
them, update cac server SVR314 SVR283 SVR225L
</commit_message>
<xml_diff>
--- a/Tong hop svr  21-10-2013.xls.xlsx
+++ b/Tong hop svr  21-10-2013.xls.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10924" uniqueCount="4352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10928" uniqueCount="4356">
   <si>
     <t>222.255.27.129</t>
   </si>
@@ -14493,9 +14493,6 @@
     <t> portal server</t>
   </si>
   <si>
-    <t> NT – VCM</t>
-  </si>
-  <si>
     <t>250.130</t>
   </si>
   <si>
@@ -14554,6 +14551,21 @@
       </rPr>
       <t>550W SP552-2C</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> NT </t>
+  </si>
+  <si>
+    <t>123.30.53.121</t>
+  </si>
+  <si>
+    <t>GSM - Teamtop</t>
+  </si>
+  <si>
+    <t>CPU 4 Core/ Ram 4GB/ HDD 40GB + 120GB</t>
+  </si>
+  <si>
+    <t>W2k3 32</t>
   </si>
 </sst>
 </file>
@@ -17045,6 +17057,9 @@
     </xf>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -17125,9 +17140,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -17655,9 +17667,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:IQ1261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A351" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P371" sqref="P371"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A363" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H373" sqref="H373"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17681,24 +17693,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:251" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="686" t="s">
+      <c r="A1" s="687" t="s">
         <v>2477</v>
       </c>
-      <c r="B1" s="687"/>
-      <c r="C1" s="687"/>
-      <c r="D1" s="687"/>
-      <c r="E1" s="687"/>
-      <c r="F1" s="687"/>
-      <c r="G1" s="687"/>
-      <c r="H1" s="687"/>
-      <c r="I1" s="687"/>
-      <c r="J1" s="687"/>
-      <c r="K1" s="687"/>
-      <c r="L1" s="687"/>
-      <c r="M1" s="687"/>
-      <c r="N1" s="687"/>
-      <c r="O1" s="687"/>
-      <c r="P1" s="687"/>
+      <c r="B1" s="688"/>
+      <c r="C1" s="688"/>
+      <c r="D1" s="688"/>
+      <c r="E1" s="688"/>
+      <c r="F1" s="688"/>
+      <c r="G1" s="688"/>
+      <c r="H1" s="688"/>
+      <c r="I1" s="688"/>
+      <c r="J1" s="688"/>
+      <c r="K1" s="688"/>
+      <c r="L1" s="688"/>
+      <c r="M1" s="688"/>
+      <c r="N1" s="688"/>
+      <c r="O1" s="688"/>
+      <c r="P1" s="688"/>
     </row>
     <row r="2" spans="1:251" s="301" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="537" t="s">
@@ -17749,8 +17761,8 @@
       <c r="P2" s="534" t="s">
         <v>2486</v>
       </c>
-      <c r="Q2" s="715" t="s">
-        <v>4349</v>
+      <c r="Q2" s="686" t="s">
+        <v>4348</v>
       </c>
       <c r="IP2" s="428"/>
       <c r="IQ2" s="428"/>
@@ -32158,13 +32170,13 @@
         <v>764</v>
       </c>
       <c r="D371" s="50" t="s">
+        <v>4337</v>
+      </c>
+      <c r="E371" s="50" t="s">
+        <v>4336</v>
+      </c>
+      <c r="F371" s="50" t="s">
         <v>4338</v>
-      </c>
-      <c r="E371" s="50" t="s">
-        <v>4337</v>
-      </c>
-      <c r="F371" s="50" t="s">
-        <v>4339</v>
       </c>
       <c r="G371" s="85" t="s">
         <v>1824</v>
@@ -32179,13 +32191,13 @@
       </c>
       <c r="N371" s="50"/>
       <c r="O371" s="50" t="s">
-        <v>4340</v>
+        <v>4339</v>
       </c>
       <c r="P371" s="651" t="s">
-        <v>4351</v>
+        <v>4350</v>
       </c>
       <c r="Q371" s="3" t="s">
-        <v>4350</v>
+        <v>4349</v>
       </c>
     </row>
     <row r="372" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -32196,10 +32208,10 @@
       <c r="C372" s="85"/>
       <c r="D372" s="50"/>
       <c r="E372" s="50" t="s">
-        <v>4347</v>
+        <v>4346</v>
       </c>
       <c r="F372" s="50" t="s">
-        <v>4341</v>
+        <v>4340</v>
       </c>
       <c r="G372" s="85"/>
       <c r="H372" s="85"/>
@@ -32228,29 +32240,35 @@
       <c r="C373" s="85"/>
       <c r="D373" s="102"/>
       <c r="E373" s="50" t="s">
-        <v>4348</v>
+        <v>4347</v>
       </c>
       <c r="F373" s="102" t="s">
-        <v>4342</v>
-      </c>
-      <c r="G373" s="85"/>
-      <c r="H373" s="85"/>
+        <v>4341</v>
+      </c>
+      <c r="G373" s="85" t="s">
+        <v>4355</v>
+      </c>
+      <c r="H373" s="85" t="s">
+        <v>2572</v>
+      </c>
       <c r="I373" s="288" t="s">
         <v>735</v>
       </c>
       <c r="J373" s="288" t="s">
-        <v>735</v>
+        <v>4353</v>
       </c>
       <c r="K373" s="288" t="s">
-        <v>735</v>
+        <v>2322</v>
       </c>
       <c r="L373" s="85" t="s">
-        <v>735</v>
+        <v>2328</v>
       </c>
       <c r="M373" s="234"/>
       <c r="N373" s="50"/>
       <c r="O373" s="50"/>
-      <c r="P373" s="21"/>
+      <c r="P373" s="356" t="s">
+        <v>4354</v>
+      </c>
     </row>
     <row r="374" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A374" s="50"/>
@@ -32261,7 +32279,7 @@
       <c r="D374" s="50"/>
       <c r="E374" s="50"/>
       <c r="F374" s="102" t="s">
-        <v>4343</v>
+        <v>4342</v>
       </c>
       <c r="G374" s="85"/>
       <c r="H374" s="85"/>
@@ -32291,7 +32309,7 @@
       <c r="D375" s="50"/>
       <c r="E375" s="50"/>
       <c r="F375" s="50" t="s">
-        <v>4344</v>
+        <v>4343</v>
       </c>
       <c r="G375" s="85"/>
       <c r="H375" s="85"/>
@@ -32321,7 +32339,7 @@
       <c r="D376" s="50"/>
       <c r="E376" s="50"/>
       <c r="F376" s="50" t="s">
-        <v>4345</v>
+        <v>4344</v>
       </c>
       <c r="G376" s="85"/>
       <c r="H376" s="85"/>
@@ -32351,7 +32369,7 @@
       <c r="D377" s="50"/>
       <c r="E377" s="50"/>
       <c r="F377" s="102" t="s">
-        <v>4346</v>
+        <v>4345</v>
       </c>
       <c r="G377" s="85"/>
       <c r="H377" s="85"/>
@@ -34052,7 +34070,7 @@
         <v>4324</v>
       </c>
       <c r="O428" s="206" t="s">
-        <v>4336</v>
+        <v>4335</v>
       </c>
       <c r="P428" s="21" t="s">
         <v>4323</v>
@@ -34079,7 +34097,7 @@
         <v>4334</v>
       </c>
       <c r="J429" s="291" t="s">
-        <v>4335</v>
+        <v>4351</v>
       </c>
       <c r="K429" s="291" t="s">
         <v>155</v>
@@ -36338,7 +36356,9 @@
       <c r="C494" s="121" t="s">
         <v>48</v>
       </c>
-      <c r="D494" s="120"/>
+      <c r="D494" s="120" t="s">
+        <v>4352</v>
+      </c>
       <c r="E494" s="121"/>
       <c r="F494" s="121" t="s">
         <v>838</v>
@@ -63583,22 +63603,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:249" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="686" t="s">
+      <c r="A1" s="687" t="s">
         <v>2477</v>
       </c>
-      <c r="B1" s="687"/>
-      <c r="C1" s="687"/>
-      <c r="D1" s="687"/>
-      <c r="E1" s="687"/>
-      <c r="F1" s="687"/>
-      <c r="G1" s="687"/>
-      <c r="H1" s="687"/>
-      <c r="I1" s="687"/>
-      <c r="J1" s="687"/>
-      <c r="K1" s="687"/>
-      <c r="L1" s="687"/>
-      <c r="M1" s="687"/>
-      <c r="N1" s="687"/>
+      <c r="B1" s="688"/>
+      <c r="C1" s="688"/>
+      <c r="D1" s="688"/>
+      <c r="E1" s="688"/>
+      <c r="F1" s="688"/>
+      <c r="G1" s="688"/>
+      <c r="H1" s="688"/>
+      <c r="I1" s="688"/>
+      <c r="J1" s="688"/>
+      <c r="K1" s="688"/>
+      <c r="L1" s="688"/>
+      <c r="M1" s="688"/>
+      <c r="N1" s="688"/>
     </row>
     <row r="2" spans="1:249" s="301" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="537" t="s">
@@ -64159,67 +64179,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="703" t="s">
+      <c r="A1" s="704" t="s">
         <v>718</v>
       </c>
-      <c r="B1" s="705" t="s">
+      <c r="B1" s="706" t="s">
         <v>719</v>
       </c>
-      <c r="C1" s="707" t="s">
+      <c r="C1" s="708" t="s">
         <v>745</v>
       </c>
-      <c r="D1" s="707" t="s">
+      <c r="D1" s="708" t="s">
         <v>721</v>
       </c>
-      <c r="E1" s="707" t="s">
+      <c r="E1" s="708" t="s">
         <v>722</v>
       </c>
-      <c r="F1" s="701" t="s">
+      <c r="F1" s="702" t="s">
         <v>723</v>
       </c>
-      <c r="G1" s="699" t="s">
+      <c r="G1" s="700" t="s">
         <v>724</v>
       </c>
-      <c r="H1" s="699" t="s">
+      <c r="H1" s="700" t="s">
         <v>725</v>
       </c>
-      <c r="I1" s="699" t="s">
+      <c r="I1" s="700" t="s">
         <v>726</v>
       </c>
-      <c r="J1" s="699" t="s">
+      <c r="J1" s="700" t="s">
         <v>727</v>
       </c>
-      <c r="K1" s="697" t="s">
+      <c r="K1" s="698" t="s">
         <v>728</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="704"/>
-      <c r="B2" s="706"/>
-      <c r="C2" s="708"/>
-      <c r="D2" s="708"/>
-      <c r="E2" s="708"/>
-      <c r="F2" s="702"/>
-      <c r="G2" s="700"/>
-      <c r="H2" s="700"/>
-      <c r="I2" s="700"/>
-      <c r="J2" s="700"/>
-      <c r="K2" s="698"/>
+      <c r="A2" s="705"/>
+      <c r="B2" s="707"/>
+      <c r="C2" s="709"/>
+      <c r="D2" s="709"/>
+      <c r="E2" s="709"/>
+      <c r="F2" s="703"/>
+      <c r="G2" s="701"/>
+      <c r="H2" s="701"/>
+      <c r="I2" s="701"/>
+      <c r="J2" s="701"/>
+      <c r="K2" s="699"/>
     </row>
     <row r="3" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="691" t="s">
+      <c r="A3" s="692" t="s">
         <v>1885</v>
       </c>
-      <c r="B3" s="692"/>
-      <c r="C3" s="692"/>
-      <c r="D3" s="692"/>
-      <c r="E3" s="692"/>
-      <c r="F3" s="692"/>
-      <c r="G3" s="692"/>
-      <c r="H3" s="692"/>
-      <c r="I3" s="692"/>
-      <c r="J3" s="692"/>
-      <c r="K3" s="693"/>
+      <c r="B3" s="693"/>
+      <c r="C3" s="693"/>
+      <c r="D3" s="693"/>
+      <c r="E3" s="693"/>
+      <c r="F3" s="693"/>
+      <c r="G3" s="693"/>
+      <c r="H3" s="693"/>
+      <c r="I3" s="693"/>
+      <c r="J3" s="693"/>
+      <c r="K3" s="694"/>
     </row>
     <row r="4" spans="1:11" s="12" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="350">
@@ -64277,19 +64297,19 @@
       <c r="K6" s="61"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="694" t="s">
+      <c r="A7" s="695" t="s">
         <v>1802</v>
       </c>
-      <c r="B7" s="695"/>
-      <c r="C7" s="695"/>
-      <c r="D7" s="695"/>
-      <c r="E7" s="695"/>
-      <c r="F7" s="695"/>
-      <c r="G7" s="695"/>
-      <c r="H7" s="695"/>
-      <c r="I7" s="695"/>
-      <c r="J7" s="695"/>
-      <c r="K7" s="696"/>
+      <c r="B7" s="696"/>
+      <c r="C7" s="696"/>
+      <c r="D7" s="696"/>
+      <c r="E7" s="696"/>
+      <c r="F7" s="696"/>
+      <c r="G7" s="696"/>
+      <c r="H7" s="696"/>
+      <c r="I7" s="696"/>
+      <c r="J7" s="696"/>
+      <c r="K7" s="697"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="61"/>
@@ -64328,19 +64348,19 @@
       <c r="K9" s="61"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="694" t="s">
+      <c r="A10" s="695" t="s">
         <v>1807</v>
       </c>
-      <c r="B10" s="695"/>
-      <c r="C10" s="695"/>
-      <c r="D10" s="695"/>
-      <c r="E10" s="695"/>
-      <c r="F10" s="695"/>
-      <c r="G10" s="695"/>
-      <c r="H10" s="695"/>
-      <c r="I10" s="695"/>
-      <c r="J10" s="695"/>
-      <c r="K10" s="696"/>
+      <c r="B10" s="696"/>
+      <c r="C10" s="696"/>
+      <c r="D10" s="696"/>
+      <c r="E10" s="696"/>
+      <c r="F10" s="696"/>
+      <c r="G10" s="696"/>
+      <c r="H10" s="696"/>
+      <c r="I10" s="696"/>
+      <c r="J10" s="696"/>
+      <c r="K10" s="697"/>
     </row>
     <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="61"/>
@@ -64420,19 +64440,19 @@
       <c r="K15" s="61"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="694" t="s">
+      <c r="A16" s="695" t="s">
         <v>1881</v>
       </c>
-      <c r="B16" s="695"/>
-      <c r="C16" s="695"/>
-      <c r="D16" s="695"/>
-      <c r="E16" s="695"/>
-      <c r="F16" s="695"/>
-      <c r="G16" s="695"/>
-      <c r="H16" s="695"/>
-      <c r="I16" s="695"/>
-      <c r="J16" s="695"/>
-      <c r="K16" s="696"/>
+      <c r="B16" s="696"/>
+      <c r="C16" s="696"/>
+      <c r="D16" s="696"/>
+      <c r="E16" s="696"/>
+      <c r="F16" s="696"/>
+      <c r="G16" s="696"/>
+      <c r="H16" s="696"/>
+      <c r="I16" s="696"/>
+      <c r="J16" s="696"/>
+      <c r="K16" s="697"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="61"/>
@@ -64475,19 +64495,19 @@
       <c r="K18" s="61"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="688" t="s">
+      <c r="A20" s="689" t="s">
         <v>1939</v>
       </c>
-      <c r="B20" s="689"/>
-      <c r="C20" s="689"/>
-      <c r="D20" s="689"/>
-      <c r="E20" s="689"/>
-      <c r="F20" s="689"/>
-      <c r="G20" s="689"/>
-      <c r="H20" s="689"/>
-      <c r="I20" s="689"/>
-      <c r="J20" s="689"/>
-      <c r="K20" s="690"/>
+      <c r="B20" s="690"/>
+      <c r="C20" s="690"/>
+      <c r="D20" s="690"/>
+      <c r="E20" s="690"/>
+      <c r="F20" s="690"/>
+      <c r="G20" s="690"/>
+      <c r="H20" s="690"/>
+      <c r="I20" s="690"/>
+      <c r="J20" s="690"/>
+      <c r="K20" s="691"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="61"/>
@@ -64583,52 +64603,52 @@
       <c r="F3"/>
     </row>
     <row r="4" spans="1:13" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="709" t="s">
+      <c r="A4" s="710" t="s">
         <v>718</v>
       </c>
-      <c r="B4" s="710" t="s">
+      <c r="B4" s="711" t="s">
         <v>719</v>
       </c>
-      <c r="C4" s="711" t="s">
+      <c r="C4" s="712" t="s">
         <v>720</v>
       </c>
-      <c r="D4" s="711" t="s">
+      <c r="D4" s="712" t="s">
         <v>506</v>
       </c>
-      <c r="E4" s="711" t="s">
+      <c r="E4" s="712" t="s">
         <v>507</v>
       </c>
-      <c r="F4" s="714" t="s">
+      <c r="F4" s="715" t="s">
         <v>723</v>
       </c>
-      <c r="G4" s="712" t="s">
+      <c r="G4" s="713" t="s">
         <v>724</v>
       </c>
-      <c r="H4" s="712" t="s">
+      <c r="H4" s="713" t="s">
         <v>725</v>
       </c>
-      <c r="I4" s="712" t="s">
+      <c r="I4" s="713" t="s">
         <v>726</v>
       </c>
-      <c r="J4" s="711" t="s">
+      <c r="J4" s="712" t="s">
         <v>508</v>
       </c>
-      <c r="K4" s="713" t="s">
+      <c r="K4" s="714" t="s">
         <v>728</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="709"/>
-      <c r="B5" s="710"/>
-      <c r="C5" s="711"/>
-      <c r="D5" s="711"/>
-      <c r="E5" s="711"/>
-      <c r="F5" s="714"/>
-      <c r="G5" s="712"/>
-      <c r="H5" s="712"/>
-      <c r="I5" s="712"/>
-      <c r="J5" s="711"/>
-      <c r="K5" s="713"/>
+      <c r="A5" s="710"/>
+      <c r="B5" s="711"/>
+      <c r="C5" s="712"/>
+      <c r="D5" s="712"/>
+      <c r="E5" s="712"/>
+      <c r="F5" s="715"/>
+      <c r="G5" s="713"/>
+      <c r="H5" s="713"/>
+      <c r="I5" s="713"/>
+      <c r="J5" s="712"/>
+      <c r="K5" s="714"/>
     </row>
     <row r="6" spans="1:13" s="8" customFormat="1" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="16">

</xml_diff>